<commit_message>
add the B1~B7 evidenence
</commit_message>
<xml_diff>
--- a/xavier200203/evidence.xlsx
+++ b/xavier200203/evidence.xlsx
@@ -33,13 +33,14 @@
     <sheet name="B2" sheetId="23" r:id="rId23"/>
     <sheet name="B5" sheetId="24" r:id="rId24"/>
     <sheet name="B6" sheetId="25" r:id="rId25"/>
+    <sheet name="B7" sheetId="26" r:id="rId26"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="102">
   <si>
     <t>TeamName</t>
   </si>
@@ -329,10 +330,22 @@
     <t>171861F856A142F6F35F4E22FD963DE485CD51D8FEE81D0C0B3B37CA1A0C958A</t>
   </si>
   <si>
-    <t>The first Interchain NFT-Transfer TxHash</t>
-  </si>
-  <si>
-    <t>The Internal Transfer TxHash on IRISnet</t>
+    <t>07DEB1F11A99EEFB606A78F3D25B0FE1FAC098B68BA584782C682F0889CA973E</t>
+  </si>
+  <si>
+    <t>F5CBE969587F4720D5043AACD59A3CDDCCEAE2629DC10B49F280EA71D420FF1F</t>
+  </si>
+  <si>
+    <t>44D7D05A34582F013F4E0DC44902A2BCCC109E984C40365916FE7C8FD9DC9886</t>
+  </si>
+  <si>
+    <t>F3D8789181D803EB0AAA1A405A7E002545003A7A4790B99229F77FF96C1BCF7F</t>
+  </si>
+  <si>
+    <t>78FC2D38258EC594021C8700ABCA6DB0429149BD7E95EE2521101F6CACA78A04</t>
+  </si>
+  <si>
+    <t>04923C19627F62AAD1E1F8307503043AD84F26B58E8DE8FB2407EA9E5E743BC7</t>
   </si>
 </sst>
 </file>
@@ -340,10 +353,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="177" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="178" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="179" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="179" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="32">
     <font>
@@ -363,6 +376,12 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <charset val="134"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF24292F"/>
+      <name val="Helvetica"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
@@ -372,12 +391,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color rgb="FF24292F"/>
-      <name val="Helvetica"/>
-      <charset val="1"/>
-    </font>
-    <font>
       <sz val="11"/>
       <name val="宋体"/>
       <charset val="134"/>
@@ -418,9 +431,63 @@
       <charset val="1"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="10"/>
       <name val="Arial"/>
       <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <b/>
@@ -431,6 +498,73 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="13"/>
       <color theme="3"/>
@@ -440,132 +574,11 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="35">
     <fill>
@@ -588,37 +601,133 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -630,145 +739,49 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -779,6 +792,15 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -797,15 +819,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -817,15 +830,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -854,17 +858,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -879,141 +872,161 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="15" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="15" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="9" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="13" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="10" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="9" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="13" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="13" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="13" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="7" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="8" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="12" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="22" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="11" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="8" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="12" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="12" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="12" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="12" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="9" fontId="13" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1022,13 +1035,14 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1036,7 +1050,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1445,9 +1458,9 @@
   <sheetFormatPr defaultColWidth="12.6428571428571" defaultRowHeight="12" outlineLevelRow="1" outlineLevelCol="7"/>
   <cols>
     <col min="1" max="1" width="14.6160714285714" customWidth="1"/>
-    <col min="2" max="2" width="14.8839285714286" customWidth="1"/>
-    <col min="3" max="3" width="17.5089285714286" customWidth="1"/>
-    <col min="4" max="4" width="16.1339285714286" customWidth="1"/>
+    <col min="2" max="2" width="45.2321428571429" customWidth="1"/>
+    <col min="3" max="3" width="50.7321428571429" customWidth="1"/>
+    <col min="4" max="4" width="43.4464285714286" customWidth="1"/>
     <col min="5" max="5" width="45.7142857142857" customWidth="1"/>
     <col min="6" max="6" width="17.7410714285714" customWidth="1"/>
     <col min="7" max="7" width="15.5" customWidth="1"/>
@@ -1547,7 +1560,7 @@
       <c r="A7" s="11"/>
     </row>
     <row r="9" ht="12.8" spans="1:1">
-      <c r="A9" s="10"/>
+      <c r="A9" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511811023622047" footer="0.511811023622047"/>
@@ -1580,15 +1593,15 @@
       </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" s="9" t="s">
+      <c r="A2" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="10" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="12" ht="12.8" spans="1:1">
-      <c r="A12" s="5"/>
+      <c r="A12" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511811023622047" footer="0.511811023622047"/>
@@ -1620,15 +1633,15 @@
       </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" s="9" t="s">
+      <c r="A2" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="10" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="18" ht="12.8" spans="1:1">
-      <c r="A18" s="10"/>
+      <c r="A18" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511811023622047" footer="0.511811023622047"/>
@@ -1660,18 +1673,18 @@
       </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" s="9" t="s">
+      <c r="A2" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="10" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="14" ht="12.8" spans="1:1">
-      <c r="A14" s="5"/>
+      <c r="A14" s="4"/>
     </row>
     <row r="15" spans="1:1">
-      <c r="A15" s="6"/>
+      <c r="A15" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511811023622047" footer="0.511811023622047"/>
@@ -1706,7 +1719,7 @@
       <c r="A2" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="8" t="s">
         <v>39</v>
       </c>
     </row>
@@ -1714,7 +1727,7 @@
       <c r="A3" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="8" t="s">
         <v>33</v>
       </c>
     </row>
@@ -1722,7 +1735,7 @@
       <c r="A4" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="8" t="s">
         <v>36</v>
       </c>
     </row>
@@ -1730,15 +1743,15 @@
       <c r="A5" t="s">
         <v>57</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="8" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="16" ht="12.8" spans="1:1">
-      <c r="A16" s="5"/>
+      <c r="A16" s="4"/>
     </row>
     <row r="17" spans="1:1">
-      <c r="A17" s="6"/>
+      <c r="A17" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511811023622047" footer="0.511811023622047"/>
@@ -1773,7 +1786,7 @@
       <c r="A2" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="9" t="s">
         <v>39</v>
       </c>
     </row>
@@ -1781,7 +1794,7 @@
       <c r="A3" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="9" t="s">
         <v>36</v>
       </c>
     </row>
@@ -1789,7 +1802,7 @@
       <c r="A4" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="9" t="s">
         <v>61</v>
       </c>
     </row>
@@ -1797,15 +1810,15 @@
       <c r="A5" t="s">
         <v>62</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="9" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="15" ht="12.8" spans="1:1">
-      <c r="A15" s="5"/>
+      <c r="A15" s="4"/>
     </row>
     <row r="16" spans="1:1">
-      <c r="A16" s="6"/>
+      <c r="A16" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511811023622047" footer="0.511811023622047"/>
@@ -1840,7 +1853,7 @@
       <c r="A2" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="7" t="s">
         <v>39</v>
       </c>
     </row>
@@ -1848,7 +1861,7 @@
       <c r="A3" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="7" t="s">
         <v>65</v>
       </c>
     </row>
@@ -1856,7 +1869,7 @@
       <c r="A4" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="7" t="s">
         <v>36</v>
       </c>
     </row>
@@ -1864,15 +1877,15 @@
       <c r="A5" t="s">
         <v>67</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="7" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="14" ht="12.8" spans="1:1">
-      <c r="A14" s="5"/>
+      <c r="A14" s="4"/>
     </row>
     <row r="15" spans="1:1">
-      <c r="A15" s="6"/>
+      <c r="A15" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511811023622047" footer="0.511811023622047"/>
@@ -1907,7 +1920,7 @@
       <c r="A2" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="7" t="s">
         <v>39</v>
       </c>
     </row>
@@ -1915,7 +1928,7 @@
       <c r="A3" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="7" t="s">
         <v>65</v>
       </c>
     </row>
@@ -1923,7 +1936,7 @@
       <c r="A4" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="8" t="s">
         <v>33</v>
       </c>
     </row>
@@ -1931,15 +1944,15 @@
       <c r="A5" t="s">
         <v>71</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="7" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="14" ht="12.8" spans="1:1">
-      <c r="A14" s="5"/>
+      <c r="A14" s="4"/>
     </row>
     <row r="15" spans="1:1">
-      <c r="A15" s="6"/>
+      <c r="A15" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511811023622047" footer="0.511811023622047"/>
@@ -1974,7 +1987,7 @@
       <c r="A2" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="7" t="s">
         <v>39</v>
       </c>
     </row>
@@ -1982,7 +1995,7 @@
       <c r="A3" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="8" t="s">
         <v>33</v>
       </c>
     </row>
@@ -1990,7 +2003,7 @@
       <c r="A4" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="7" t="s">
         <v>65</v>
       </c>
     </row>
@@ -1998,15 +2011,15 @@
       <c r="A5" t="s">
         <v>75</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="8" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="12" ht="12.8" spans="1:1">
-      <c r="A12" s="5"/>
+      <c r="A12" s="4"/>
     </row>
     <row r="13" spans="1:1">
-      <c r="A13" s="6"/>
+      <c r="A13" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511811023622047" footer="0.511811023622047"/>
@@ -2041,7 +2054,7 @@
       <c r="A2" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="7" t="s">
         <v>39</v>
       </c>
     </row>
@@ -2049,7 +2062,7 @@
       <c r="A3" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="7" t="s">
         <v>61</v>
       </c>
     </row>
@@ -2057,7 +2070,7 @@
       <c r="A4" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="7" t="s">
         <v>36</v>
       </c>
     </row>
@@ -2065,15 +2078,15 @@
       <c r="A5" t="s">
         <v>79</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="7" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="14" ht="12.8" spans="1:1">
-      <c r="A14" s="5"/>
+      <c r="A14" s="4"/>
     </row>
     <row r="15" spans="1:1">
-      <c r="A15" s="6"/>
+      <c r="A15" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511811023622047" footer="0.511811023622047"/>
@@ -2088,12 +2101,13 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6428571428571" defaultRowHeight="12" outlineLevelRow="1" outlineLevelCol="1"/>
   <cols>
-    <col min="1" max="2" width="17.8839285714286" customWidth="1"/>
+    <col min="1" max="1" width="97.9196428571429" customWidth="1"/>
+    <col min="2" max="2" width="76.7857142857143" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="13.2" spans="1:2">
@@ -2145,7 +2159,7 @@
       <c r="A2" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="7" t="s">
         <v>39</v>
       </c>
     </row>
@@ -2153,7 +2167,7 @@
       <c r="A3" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="7" t="s">
         <v>33</v>
       </c>
     </row>
@@ -2161,7 +2175,7 @@
       <c r="A4" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="7" t="s">
         <v>65</v>
       </c>
     </row>
@@ -2169,7 +2183,7 @@
       <c r="A5" t="s">
         <v>83</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="7" t="s">
         <v>36</v>
       </c>
     </row>
@@ -2177,7 +2191,7 @@
       <c r="A6" t="s">
         <v>84</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="7" t="s">
         <v>65</v>
       </c>
     </row>
@@ -2185,15 +2199,15 @@
       <c r="A7" t="s">
         <v>85</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="7" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="13" ht="12.8" spans="1:1">
-      <c r="A13" s="5"/>
+      <c r="A13" s="4"/>
     </row>
     <row r="14" spans="1:1">
-      <c r="A14" s="6"/>
+      <c r="A14" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511811023622047" footer="0.511811023622047"/>
@@ -2228,7 +2242,7 @@
       <c r="A2" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="7" t="s">
         <v>39</v>
       </c>
     </row>
@@ -2236,7 +2250,7 @@
       <c r="A3" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="7" t="s">
         <v>36</v>
       </c>
     </row>
@@ -2244,7 +2258,7 @@
       <c r="A4" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="7" t="s">
         <v>33</v>
       </c>
     </row>
@@ -2252,7 +2266,7 @@
       <c r="A5" t="s">
         <v>89</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="7" t="s">
         <v>61</v>
       </c>
     </row>
@@ -2260,7 +2274,7 @@
       <c r="A6" t="s">
         <v>90</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="7" t="s">
         <v>33</v>
       </c>
     </row>
@@ -2268,12 +2282,12 @@
       <c r="A7" t="s">
         <v>91</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="7" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="14" ht="12.8" spans="1:1">
-      <c r="A14" s="5"/>
+      <c r="A14" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511811023622047" footer="0.511811023622047"/>
@@ -2357,13 +2371,16 @@
 <file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:A3"/>
+  <dimension ref="A1:A9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5357142857143" defaultRowHeight="12" outlineLevelRow="2"/>
+  <sheetFormatPr defaultColWidth="11.5357142857143" defaultRowHeight="12"/>
+  <cols>
+    <col min="1" max="1" width="82.2857142857143" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" ht="13.2" spans="1:1">
       <c r="A1" s="1" t="s">
@@ -2379,6 +2396,9 @@
       <c r="A3" s="3" t="s">
         <v>97</v>
       </c>
+    </row>
+    <row r="9" ht="12.8" spans="1:1">
+      <c r="A9" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -2393,13 +2413,16 @@
 <file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:A3"/>
+  <dimension ref="A1:A12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5357142857143" defaultRowHeight="12" outlineLevelRow="2"/>
+  <sheetFormatPr defaultColWidth="11.5357142857143" defaultRowHeight="12"/>
+  <cols>
+    <col min="1" max="1" width="78.2678571428571" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" ht="13.2" spans="1:1">
       <c r="A1" s="1" t="s">
@@ -2408,13 +2431,64 @@
     </row>
     <row r="2" ht="13.2" spans="1:1">
       <c r="A2" s="2" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
     </row>
     <row r="3" ht="13.2" spans="1:1">
       <c r="A3" s="3" t="s">
-        <v>97</v>
-      </c>
+        <v>99</v>
+      </c>
+    </row>
+    <row r="11" ht="12.8" spans="1:1">
+      <c r="A11" s="4"/>
+    </row>
+    <row r="12" spans="1:1">
+      <c r="A12" s="5"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <headerFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;Kffffff&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;KffffffPage &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:A11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.5357142857143" defaultRowHeight="12"/>
+  <cols>
+    <col min="1" max="1" width="86.0089285714286" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="13.2" spans="1:1">
+      <c r="A1" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" ht="13.2" spans="1:1">
+      <c r="A2" s="2" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3" ht="13.2" spans="1:1">
+      <c r="A3" s="3" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="10" ht="12.8" spans="1:1">
+      <c r="A10" s="4"/>
+    </row>
+    <row r="11" spans="1:1">
+      <c r="A11" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -2487,13 +2561,13 @@
       </c>
     </row>
     <row r="5" spans="1:3">
-      <c r="A5" s="9" t="s">
+      <c r="A5" s="10" t="s">
         <v>27</v>
       </c>
       <c r="B5" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="C5" s="9" t="s">
+      <c r="C5" s="10" t="s">
         <v>28</v>
       </c>
     </row>
@@ -2594,13 +2668,13 @@
       </c>
     </row>
     <row r="2" spans="1:4">
-      <c r="A2" s="9" t="s">
+      <c r="A2" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="C2" s="9" t="s">
+      <c r="C2" s="10" t="s">
         <v>28</v>
       </c>
       <c r="D2" s="13" t="s">
@@ -2646,13 +2720,13 @@
       </c>
     </row>
     <row r="2" spans="1:4">
-      <c r="A2" s="9" t="s">
+      <c r="A2" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="C2" s="9" t="s">
+      <c r="C2" s="10" t="s">
         <v>26</v>
       </c>
       <c r="D2" s="13" t="s">
@@ -2698,13 +2772,13 @@
       </c>
     </row>
     <row r="2" spans="1:4">
-      <c r="A2" s="9" t="s">
+      <c r="A2" s="10" t="s">
         <v>40</v>
       </c>
       <c r="B2" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="C2" s="9" t="s">
+      <c r="C2" s="10" t="s">
         <v>28</v>
       </c>
       <c r="D2" s="13" t="s">
@@ -2749,7 +2823,7 @@
       </c>
     </row>
     <row r="11" ht="12.8" spans="1:1">
-      <c r="A11" s="10" t="s">
+      <c r="A11" s="6" t="s">
         <v>43</v>
       </c>
     </row>
@@ -2797,7 +2871,7 @@
       </c>
     </row>
     <row r="9" ht="12.8" spans="1:1">
-      <c r="A9" s="10" t="s">
+      <c r="A9" s="6" t="s">
         <v>43</v>
       </c>
     </row>

</xml_diff>